<commit_message>
Add latest data sheet.
</commit_message>
<xml_diff>
--- a/data/Semester 1 Simulated Timetable_20200629.xlsx
+++ b/data/Semester 1 Simulated Timetable_20200629.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Macintosh/github/OpenClassroom/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39183E83-EFA1-D84E-9FDA-78B166960C04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C79DD85-A92D-0B4F-8F66-272B123BC8BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16860" yWindow="0" windowWidth="21540" windowHeight="21600" tabRatio="870" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="870" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL" sheetId="1" r:id="rId1"/>
@@ -64094,9 +64094,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -64232,19 +64235,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A73741E-3D25-46A0-B941-3BCE797C8614}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5780C669-9F48-4986-A2B0-9CCE7D434435}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -64268,9 +64267,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5780C669-9F48-4986-A2B0-9CCE7D434435}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A73741E-3D25-46A0-B941-3BCE797C8614}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>